<commit_message>
Add customer measurements and BMI information and calculations for male
</commit_message>
<xml_diff>
--- a/BMI Measurement methods.xlsx
+++ b/BMI Measurement methods.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/igorjacon/Development/Symfony/terra_nutrition_web_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E845A33-874A-2B4D-826A-DB3E5945CB8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9685D78-0B38-3C44-BDCA-AFC8CA995E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" xr2:uid="{D629F377-0FF2-014F-9C86-B285B1FBC4E0}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16140" xr2:uid="{D629F377-0FF2-014F-9C86-B285B1FBC4E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Jackson &amp; Pollock Method" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -465,7 +465,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -518,37 +518,37 @@
         <v>48</v>
       </c>
       <c r="B2" s="1">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C2" s="1">
-        <v>1.71</v>
+        <v>1.59</v>
       </c>
       <c r="D2" s="1">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E2" s="2">
         <f>D2/(C2^2)</f>
-        <v>21.887076365377382</v>
+        <v>21.75546853368142</v>
       </c>
       <c r="F2" s="1">
         <f>1.0994921 - (0.0009929 * A2) + (0.0000023 * A2^2) - (0.0001392 * B2)</f>
-        <v>1.0517033</v>
+        <v>1.0529561000000001</v>
       </c>
       <c r="G2" s="1">
         <f>(495/F2) - 450</f>
-        <v>20.665063045822876</v>
+        <v>20.105068957765639</v>
       </c>
       <c r="H2" s="1">
         <f>100-G2</f>
-        <v>79.334936954177124</v>
+        <v>79.894931042234361</v>
       </c>
       <c r="I2" s="1">
         <f>(G2/100)*D2</f>
-        <v>13.225640349326641</v>
+        <v>11.0577879267711</v>
       </c>
       <c r="J2" s="1">
         <f>D2-I2</f>
-        <v>50.774359650673361</v>
+        <v>43.942212073228902</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>7</v>

</xml_diff>